<commit_message>
Added GRU results, slight improvements
</commit_message>
<xml_diff>
--- a/risultati assigment 2.xlsx
+++ b/risultati assigment 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neo Dom-Z Mk. II\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\Desktop\NLP\NLP-Assigments-22-23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DD379D-642D-47B2-A975-DEC64F4BE09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094D54BE-51A1-4D4E-A2B5-6AA0C2D88AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="1290" windowWidth="21555" windowHeight="12450" xr2:uid="{D1A9DF2D-FBE7-40F2-963C-202F180806A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1A9DF2D-FBE7-40F2-963C-202F180806A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>Encoder</t>
   </si>
@@ -111,13 +111,28 @@
   </si>
   <si>
     <t>{'exact_match': 11.667209832860003, 'f1': 14.032409258275385}</t>
+  </si>
+  <si>
+    <t>128 GRU units</t>
+  </si>
+  <si>
+    <t>101 embedding dim</t>
+  </si>
+  <si>
+    <t>102 embedding dim</t>
+  </si>
+  <si>
+    <t>103 embedding dim</t>
+  </si>
+  <si>
+    <t>{'exact_match': 12.039666651147632, 'f1': 14.165593903763927}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +157,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -532,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315EC485-42C7-4C81-92D8-9DFFE06132F7}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,19 +717,42 @@
         <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="J5" s="1">
         <v>0.76890534162521296</v>
       </c>
       <c r="K5" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -717,7 +761,8 @@
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="L2:L4"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>